<commit_message>
Update clases de Departamentos y Municipios
</commit_message>
<xml_diff>
--- a/Config/app/static/resources/departamentos.xlsx
+++ b/Config/app/static/resources/departamentos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aprendiz Sena\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aprendiz Sena\Documents\GitHub\Adso\Config\app\static\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3E57E1-62A9-4C67-9314-52F52B4266CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CCEB5AA-5C77-4CB2-BF98-5E6F18FE7E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1A732570-D614-4A99-AEF9-3C579D96B5D8}"/>
   </bookViews>
@@ -981,7 +981,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>